<commit_message>
Ajout des fichiers générés utiles.
</commit_message>
<xml_diff>
--- a/AA.xlsx
+++ b/AA.xlsx
@@ -12,24 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Semaine : </t>
   </si>
   <si>
-    <t>lundi</t>
+    <t>mardi</t>
   </si>
   <si>
-    <t>Cloud - C (KRTA9AA3)</t>
+    <t>Cloud - C (KRTA9AA3/KUPT9BB1)</t>
   </si>
   <si>
-    <t>KRTA9AA3</t>
+    <t>KRTA9AA3/KUPT9BB1</t>
   </si>
   <si>
     <t>AA</t>
   </si>
   <si>
     <t>10:0</t>
+  </si>
+  <si>
+    <t>U3-106</t>
   </si>
   <si>
     <t>TYPE_COURS</t>
@@ -90,12 +93,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="n" s="0">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="1">
-        <v>45957.0</v>
+        <v>45951.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>1</v>
@@ -117,10 +120,12 @@
       <c r="E3" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F3" s="0"/>
+      <c r="F3" t="s" s="0">
+        <v>6</v>
+      </c>
       <c r="G3" s="0"/>
       <c r="H3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="0"/>
     </row>

</xml_diff>